<commit_message>
04/02 Pushing to Meenaa Branch
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
+++ b/src/test/resources/TestData/Excel_Login_Pythoncode.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
@@ -210,7 +210,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -239,12 +239,6 @@
       <name val="Times New Roman"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -330,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -397,10 +391,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -660,7 +650,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.43"/>
@@ -28715,13 +28705,13 @@
   </sheetPr>
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="101"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="48.43"/>
@@ -56792,11 +56782,11 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="28.73"/>
   </cols>
@@ -56908,7 +56898,7 @@
       <c r="B4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D4" s="3"/>

</xml_diff>